<commit_message>
#815 - Phase accordion
</commit_message>
<xml_diff>
--- a/reports-api/src/reports_api/templates/event_templates/001-Event-Template.xlsx
+++ b/reports-api/src/reports_api/templates/event_templates/001-Event-Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aot\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\reports-api\src\reports_api\templates\event_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C335A94-FE46-462D-A285-F41CBD837A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5CC6BD-FA9A-4F55-8CED-2A1524CEE2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A853713A-B735-4946-989C-636E29001BC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{A853713A-B735-4946-989C-636E29001BC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -651,20 +649,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C810C-8C59-436D-942F-1E4DCF6E7DB1}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -690,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -716,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -751,23 +749,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153731F1-A4DA-4C0A-A099-407D72EC11B0}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -802,7 +800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -825,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -834,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -860,7 +858,7 @@
         <v>7</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -869,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -895,7 +893,7 @@
         <v>7</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -904,7 +902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -936,7 +934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -962,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -971,7 +969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -997,7 +995,7 @@
         <v>73</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -1006,7 +1004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1029,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
@@ -1038,7 +1036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1064,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -1073,7 +1071,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1099,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -1108,7 +1106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1131,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -1140,7 +1138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1166,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -1175,7 +1173,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1201,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -1210,7 +1208,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1233,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="b">
         <v>0</v>
@@ -1242,7 +1240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1265,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="b">
         <v>0</v>
@@ -1274,7 +1272,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1297,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
@@ -1306,7 +1304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1332,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="b">
         <v>0</v>
@@ -1341,7 +1339,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1367,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="b">
         <v>0</v>
@@ -1376,7 +1374,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1399,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="b">
         <v>0</v>
@@ -1408,7 +1406,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1434,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="b">
         <v>0</v>
@@ -1443,7 +1441,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1469,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="b">
         <v>0</v>
@@ -1478,7 +1476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1501,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="b">
         <v>0</v>
@@ -1510,7 +1508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1536,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="b">
         <v>0</v>
@@ -1545,7 +1543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1571,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="b">
         <v>0</v>
@@ -1580,7 +1578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1603,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="b">
         <v>0</v>
@@ -1612,7 +1610,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1638,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="b">
         <v>0</v>
@@ -1647,7 +1645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1673,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="b">
         <v>0</v>
@@ -1682,7 +1680,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1705,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="b">
         <v>0</v>
@@ -1714,7 +1712,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1740,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="b">
         <v>0</v>
@@ -1749,7 +1747,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1775,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="b">
         <v>0</v>
@@ -1784,7 +1782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1807,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="b">
         <v>0</v>
@@ -1816,7 +1814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1842,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="b">
         <v>0</v>
@@ -1851,7 +1849,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1877,7 +1875,7 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="b">
         <v>0</v>
@@ -1886,7 +1884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1909,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="b">
         <v>0</v>
@@ -1918,7 +1916,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1941,7 +1939,7 @@
         <v>50</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="b">
         <v>1</v>
@@ -1950,7 +1948,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1973,7 +1971,7 @@
         <v>5</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="b">
         <v>1</v>
@@ -1982,7 +1980,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2008,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="b">
         <v>1</v>
@@ -2017,7 +2015,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2040,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="b">
         <v>0</v>
@@ -2049,7 +2047,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2072,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="b">
         <v>0</v>
@@ -2081,7 +2079,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2107,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="b">
         <v>0</v>
@@ -2116,7 +2114,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2142,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="b">
         <v>0</v>
@@ -2151,7 +2149,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2174,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="b">
         <v>0</v>
@@ -2183,7 +2181,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2209,7 +2207,7 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="b">
         <v>0</v>
@@ -2218,7 +2216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2244,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="b">
         <v>0</v>
@@ -2253,7 +2251,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2276,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="b">
         <v>0</v>
@@ -2285,7 +2283,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2311,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" t="b">
         <v>0</v>
@@ -2320,7 +2318,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2346,7 +2344,7 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="b">
         <v>0</v>
@@ -2355,7 +2353,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2378,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="b">
         <v>0</v>
@@ -2387,7 +2385,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2413,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="b">
         <v>0</v>
@@ -2422,7 +2420,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2448,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="b">
         <v>0</v>
@@ -2457,7 +2455,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2480,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="I51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51" t="b">
         <v>0</v>
@@ -2489,7 +2487,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2515,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="I52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" t="b">
         <v>0</v>
@@ -2524,7 +2522,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2550,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="I53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" t="b">
         <v>0</v>
@@ -2559,7 +2557,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2582,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J54" t="b">
         <v>0</v>
@@ -2591,7 +2589,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2614,7 +2612,7 @@
         <v>10</v>
       </c>
       <c r="I55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J55" t="b">
         <v>1</v>
@@ -2623,7 +2621,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2649,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J56" t="b">
         <v>1</v>
@@ -2658,7 +2656,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2684,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
815 - Phase accordion (#856)
* conflicts resolved

* conflicts resolved

* #815 - Phase accordion
</commit_message>
<xml_diff>
--- a/reports-api/src/reports_api/templates/event_templates/001-Event-Template.xlsx
+++ b/reports-api/src/reports_api/templates/event_templates/001-Event-Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aot\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\reports-api\src\reports_api\templates\event_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C335A94-FE46-462D-A285-F41CBD837A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5CC6BD-FA9A-4F55-8CED-2A1524CEE2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A853713A-B735-4946-989C-636E29001BC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{A853713A-B735-4946-989C-636E29001BC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -651,20 +649,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C810C-8C59-436D-942F-1E4DCF6E7DB1}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -690,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -716,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -751,23 +749,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153731F1-A4DA-4C0A-A099-407D72EC11B0}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -802,7 +800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -825,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -834,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -860,7 +858,7 @@
         <v>7</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -869,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -895,7 +893,7 @@
         <v>7</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -904,7 +902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -936,7 +934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -962,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -971,7 +969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -997,7 +995,7 @@
         <v>73</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -1006,7 +1004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1029,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
@@ -1038,7 +1036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1064,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -1073,7 +1071,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1099,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -1108,7 +1106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1131,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -1140,7 +1138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1166,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -1175,7 +1173,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1201,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -1210,7 +1208,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1233,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="b">
         <v>0</v>
@@ -1242,7 +1240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1265,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="b">
         <v>0</v>
@@ -1274,7 +1272,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1297,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
@@ -1306,7 +1304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1332,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="b">
         <v>0</v>
@@ -1341,7 +1339,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1367,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="b">
         <v>0</v>
@@ -1376,7 +1374,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1399,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="b">
         <v>0</v>
@@ -1408,7 +1406,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1434,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="b">
         <v>0</v>
@@ -1443,7 +1441,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1469,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="b">
         <v>0</v>
@@ -1478,7 +1476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1501,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="b">
         <v>0</v>
@@ -1510,7 +1508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1536,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="b">
         <v>0</v>
@@ -1545,7 +1543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1571,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="b">
         <v>0</v>
@@ -1580,7 +1578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1603,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="b">
         <v>0</v>
@@ -1612,7 +1610,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1638,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="b">
         <v>0</v>
@@ -1647,7 +1645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1673,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="b">
         <v>0</v>
@@ -1682,7 +1680,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1705,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="b">
         <v>0</v>
@@ -1714,7 +1712,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1740,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="b">
         <v>0</v>
@@ -1749,7 +1747,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1775,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="b">
         <v>0</v>
@@ -1784,7 +1782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1807,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="b">
         <v>0</v>
@@ -1816,7 +1814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1842,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="b">
         <v>0</v>
@@ -1851,7 +1849,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1877,7 +1875,7 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="b">
         <v>0</v>
@@ -1886,7 +1884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1909,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="b">
         <v>0</v>
@@ -1918,7 +1916,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1941,7 +1939,7 @@
         <v>50</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="b">
         <v>1</v>
@@ -1950,7 +1948,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1973,7 +1971,7 @@
         <v>5</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="b">
         <v>1</v>
@@ -1982,7 +1980,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2008,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="b">
         <v>1</v>
@@ -2017,7 +2015,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2040,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="b">
         <v>0</v>
@@ -2049,7 +2047,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2072,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="b">
         <v>0</v>
@@ -2081,7 +2079,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2107,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="b">
         <v>0</v>
@@ -2116,7 +2114,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2142,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="b">
         <v>0</v>
@@ -2151,7 +2149,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2174,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="b">
         <v>0</v>
@@ -2183,7 +2181,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2209,7 +2207,7 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="b">
         <v>0</v>
@@ -2218,7 +2216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2244,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="b">
         <v>0</v>
@@ -2253,7 +2251,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2276,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="b">
         <v>0</v>
@@ -2285,7 +2283,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2311,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" t="b">
         <v>0</v>
@@ -2320,7 +2318,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2346,7 +2344,7 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="b">
         <v>0</v>
@@ -2355,7 +2353,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2378,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="b">
         <v>0</v>
@@ -2387,7 +2385,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2413,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="b">
         <v>0</v>
@@ -2422,7 +2420,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2448,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="b">
         <v>0</v>
@@ -2457,7 +2455,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2480,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="I51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51" t="b">
         <v>0</v>
@@ -2489,7 +2487,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2515,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="I52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" t="b">
         <v>0</v>
@@ -2524,7 +2522,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2550,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="I53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" t="b">
         <v>0</v>
@@ -2559,7 +2557,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2582,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J54" t="b">
         <v>0</v>
@@ -2591,7 +2589,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2614,7 +2612,7 @@
         <v>10</v>
       </c>
       <c r="I55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J55" t="b">
         <v>1</v>
@@ -2623,7 +2621,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2649,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J56" t="b">
         <v>1</v>
@@ -2658,7 +2656,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2684,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" t="b">
         <v>1</v>

</xml_diff>